<commit_message>
Registro de defectos final
</commit_message>
<xml_diff>
--- a/Prueba 2/Registro de Defectos.xlsx
+++ b/Prueba 2/Registro de Defectos.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="57">
   <si>
     <t>Reporte de Defectos</t>
   </si>
@@ -179,6 +179,24 @@
   </si>
   <si>
     <t>CP07</t>
+  </si>
+  <si>
+    <t>CP08</t>
+  </si>
+  <si>
+    <t>Creacion de objeto Carne y FrutaVerdura permite valores inferiores a 0 en cantidad y precio</t>
+  </si>
+  <si>
+    <t>Crear restricciones en métodos set que no permitan valores inferiores a 0</t>
+  </si>
+  <si>
+    <t>CP09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Objeto Carne permite ingresar categorias distintas a A-B-C </t>
+  </si>
+  <si>
+    <t>Crear restricciones que no permitan ingresar categorias fuera del modelo de negocios</t>
   </si>
 </sst>
 </file>
@@ -9800,13 +9818,13 @@
   <dimension ref="C2:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="5.28515625" customWidth="1"/>
-    <col min="4" max="4" width="82" customWidth="1"/>
+    <col min="4" max="4" width="91.85546875" customWidth="1"/>
     <col min="5" max="5" width="11.42578125" customWidth="1"/>
     <col min="8" max="8" width="84.5703125" customWidth="1"/>
   </cols>
@@ -9989,20 +10007,40 @@
       </c>
     </row>
     <row r="18" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
+      <c r="C18" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>52</v>
+      </c>
       <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
+      <c r="F18" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="19" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
+      <c r="C19" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
+      <c r="F19" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>56</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Registro de defectos corregido
Correcion ortografia
</commit_message>
<xml_diff>
--- a/Prueba 2/Registro de Defectos.xlsx
+++ b/Prueba 2/Registro de Defectos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2884d8d705fa78f8/Documentos/GitHub/CALIDAD_DE_SOFTWARE/Prueba 2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://duoccl0-my.sharepoint.com/personal/vice_zurita_duocuc_cl/Documents/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{5B315B3C-C0FB-445C-8AB7-F68F6B9E7C7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{C420395C-1786-4D7F-B55B-747C7E292174}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6C35A975-82F9-4BE7-8172-AE8AB972036F}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Registro de defectos" sheetId="4" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="59">
   <si>
     <t>Reporte de Defectos</t>
   </si>
@@ -98,55 +98,22 @@
     <t>Estado del defecto</t>
   </si>
   <si>
-    <t>Solicitado</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Crear metodo que imprima resultado de precioTotalCompra </t>
-  </si>
-  <si>
     <t>Media</t>
-  </si>
-  <si>
-    <t>Incluir el resto de los datos en el metodo</t>
   </si>
   <si>
     <t>Restringir ingreso de tipo de FrutaVerdura a la nomenclatura correspondiente de 2 letras</t>
   </si>
   <si>
-    <t xml:space="preserve">Cambiar monto estatico por parametro iva de la interfaz IMontos </t>
-  </si>
-  <si>
-    <t>Clase Producto contiene metodos que no se piden ni se usan</t>
-  </si>
-  <si>
     <t>Baja</t>
-  </si>
-  <si>
-    <t>Ingresar descuento en base a categoria</t>
-  </si>
-  <si>
-    <t>precioTotalCompra() en CarritoCompra no tiene metodo para imprimir precio</t>
   </si>
   <si>
     <t>toString() en FrutaVerdura solo muestra tipo de fruta</t>
   </si>
   <si>
-    <t>calcularMontoIva() en FrutaVerdura es realizado por un valor estatico</t>
-  </si>
-  <si>
     <t xml:space="preserve">toString() en FrutaVerdura y Producto no se pide en modelo de clases </t>
   </si>
   <si>
-    <t xml:space="preserve">Eliminar metodos </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eliminar metodos hashCode y equals </t>
-  </si>
-  <si>
     <t>setTipo() en FrutaVerdura no tiene restricciones de input</t>
-  </si>
-  <si>
-    <t>setDescuentoCategoria() en Carne obtiene valores manuamente y no en base a categoria</t>
   </si>
   <si>
     <t>Nombre proyecto: Supermercado, "Number One"</t>
@@ -156,9 +123,6 @@
   </si>
   <si>
     <t>Herramienta utilizada: NetBeans 12.4, pruebas de caja negra</t>
-  </si>
-  <si>
-    <t>Nombre alumnos: Matias Luarte - Vicente zurita</t>
   </si>
   <si>
     <t>CP01</t>
@@ -185,26 +149,68 @@
     <t>CP08</t>
   </si>
   <si>
-    <t>Creacion de objeto Carne y FrutaVerdura permite valores inferiores a 0 en cantidad y precio</t>
-  </si>
-  <si>
     <t>Crear restricciones en métodos set que no permitan valores inferiores a 0</t>
   </si>
   <si>
     <t>CP09</t>
   </si>
   <si>
-    <t xml:space="preserve">Objeto Carne permite ingresar categorias distintas a A-B-C </t>
+    <t>Datos</t>
   </si>
   <si>
-    <t>Crear restricciones que no permitan ingresar categorias fuera del modelo de negocios</t>
+    <t>Reportado</t>
+  </si>
+  <si>
+    <t>Código</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eliminar métodos </t>
+  </si>
+  <si>
+    <t>precioTotalCompra() en CarritoCompra no tiene método para imprimir precio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crear método que imprima resultado de precioTotalCompra </t>
+  </si>
+  <si>
+    <t>Incluir el resto de los datos en el método</t>
+  </si>
+  <si>
+    <t>calcularMontoIva() en FrutaVerdura es realizado por un valor estático</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cambiar monto estático por parámetro IVA de la interfaz IMontos </t>
+  </si>
+  <si>
+    <t>Clase Producto contiene métodos que no se piden ni se usan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eliminar métodos hashCode y equals </t>
+  </si>
+  <si>
+    <t>Creación de objeto Carne y FrutaVerdura permite valores inferiores a 0 en cantidad y precio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Objeto Carne permite ingresar categorías distintas a A-B-C </t>
+  </si>
+  <si>
+    <t>Crear restricciones que no permitan ingresar categorías fuera del modelo de negocios</t>
+  </si>
+  <si>
+    <t>Nombre alumnos: Matías Luarte - Vicente zurita</t>
+  </si>
+  <si>
+    <t>setDescuentoCategoria() en Carne obtiene valores manualmente y no en base a categoría</t>
+  </si>
+  <si>
+    <t>Ingresar descuento en base a categoría</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -232,6 +238,14 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -354,7 +368,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -400,6 +414,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2001,8 +2016,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4513670" y="3612810"/>
-          <a:ext cx="542271" cy="91440"/>
+          <a:off x="4242386" y="3760187"/>
+          <a:ext cx="564116" cy="91440"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2016,7 +2031,7 @@
                 <a:pt x="0" y="45720"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="542271" y="45720"/>
+                <a:pt x="564116" y="45720"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -2070,8 +2085,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="4771249" y="3644973"/>
-        <a:ext cx="27113" cy="27113"/>
+        <a:off x="4510341" y="3791804"/>
+        <a:ext cx="28205" cy="28205"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{63D76EA2-AB6F-4C79-88E3-AE5B553B1789}">
@@ -2081,8 +2096,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2388399" y="2175351"/>
-          <a:ext cx="542271" cy="1483179"/>
+          <a:off x="2031502" y="2262981"/>
+          <a:ext cx="564116" cy="1542926"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2096,13 +2111,13 @@
                 <a:pt x="0" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="271135" y="0"/>
+                <a:pt x="282058" y="0"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="271135" y="1483179"/>
+                <a:pt x="282058" y="1542926"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="542271" y="1483179"/>
+                <a:pt x="564116" y="1542926"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -2156,8 +2171,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="2620055" y="2877460"/>
-        <a:ext cx="78960" cy="78960"/>
+        <a:off x="2272490" y="2993374"/>
+        <a:ext cx="82140" cy="82140"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{4B783DBA-EE43-4B2A-93EE-8E85F82E879B}">
@@ -2167,8 +2182,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4513670" y="2871221"/>
-          <a:ext cx="542271" cy="91440"/>
+          <a:off x="4242386" y="2988724"/>
+          <a:ext cx="564116" cy="91440"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2182,7 +2197,7 @@
                 <a:pt x="0" y="45720"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="542271" y="45720"/>
+                <a:pt x="564116" y="45720"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -2236,8 +2251,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="4771249" y="2903384"/>
-        <a:ext cx="27113" cy="27113"/>
+        <a:off x="4510341" y="3020341"/>
+        <a:ext cx="28205" cy="28205"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{1DDF595E-B5B3-4F85-AC6B-7A49E82A154B}">
@@ -2247,8 +2262,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2388399" y="2175351"/>
-          <a:ext cx="542271" cy="741589"/>
+          <a:off x="2031502" y="2262981"/>
+          <a:ext cx="564116" cy="771463"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2262,13 +2277,13 @@
                 <a:pt x="0" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="271135" y="0"/>
+                <a:pt x="282058" y="0"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="271135" y="741589"/>
+                <a:pt x="282058" y="771463"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="542271" y="741589"/>
+                <a:pt x="564116" y="771463"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -2322,8 +2337,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="2636567" y="2523178"/>
-        <a:ext cx="45935" cy="45935"/>
+        <a:off x="2289667" y="2624820"/>
+        <a:ext cx="47785" cy="47785"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{A2E036C4-DBC0-4BCE-B947-7938C2FA2593}">
@@ -2333,8 +2348,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4513670" y="2129631"/>
-          <a:ext cx="542271" cy="91440"/>
+          <a:off x="4242386" y="2217261"/>
+          <a:ext cx="564116" cy="91440"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2348,13 +2363,13 @@
                 <a:pt x="0" y="45720"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="271135" y="45720"/>
+                <a:pt x="282058" y="45720"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="271135" y="77041"/>
+                <a:pt x="282058" y="78302"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="542271" y="77041"/>
+                <a:pt x="564116" y="78302"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -2408,8 +2423,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="4771227" y="2161772"/>
-        <a:ext cx="27158" cy="27158"/>
+        <a:off x="4510317" y="2248855"/>
+        <a:ext cx="28252" cy="28252"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{53650F22-90EC-4AB5-A9E6-B344371FCC88}">
@@ -2419,8 +2434,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2388399" y="2129631"/>
-          <a:ext cx="542271" cy="91440"/>
+          <a:off x="2031502" y="2217261"/>
+          <a:ext cx="564116" cy="91440"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2434,7 +2449,7 @@
                 <a:pt x="0" y="45720"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="542271" y="45720"/>
+                <a:pt x="564116" y="45720"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -2488,8 +2503,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="2645978" y="2161794"/>
-        <a:ext cx="27113" cy="27113"/>
+        <a:off x="2299457" y="2248878"/>
+        <a:ext cx="28205" cy="28205"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{9F28C4A2-411E-49A8-8BDB-315C30740BD7}">
@@ -2499,8 +2514,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4513670" y="1388041"/>
-          <a:ext cx="542271" cy="91440"/>
+          <a:off x="4242386" y="1445798"/>
+          <a:ext cx="564116" cy="91440"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2514,13 +2529,13 @@
                 <a:pt x="0" y="45720"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="271135" y="45720"/>
+                <a:pt x="282058" y="45720"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="271135" y="77041"/>
+                <a:pt x="282058" y="78302"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="542271" y="77041"/>
+                <a:pt x="564116" y="78302"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -2574,8 +2589,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="4771227" y="1420182"/>
-        <a:ext cx="27158" cy="27158"/>
+        <a:off x="4510317" y="1477392"/>
+        <a:ext cx="28252" cy="28252"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{0C412CAE-977D-4573-B83C-2529D64DCC4E}">
@@ -2585,8 +2600,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2388399" y="1433761"/>
-          <a:ext cx="542271" cy="741589"/>
+          <a:off x="2031502" y="1491518"/>
+          <a:ext cx="564116" cy="771463"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2597,16 +2612,16 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="0" y="741589"/>
+                <a:pt x="0" y="771463"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="271135" y="741589"/>
+                <a:pt x="282058" y="771463"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="271135" y="0"/>
+                <a:pt x="282058" y="0"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="542271" y="0"/>
+                <a:pt x="564116" y="0"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -2660,8 +2675,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="2636567" y="1781589"/>
-        <a:ext cx="45935" cy="45935"/>
+        <a:off x="2289667" y="1853357"/>
+        <a:ext cx="47785" cy="47785"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{8DB57F31-CF52-404E-90F4-9125356FF194}">
@@ -2671,8 +2686,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4513670" y="646452"/>
-          <a:ext cx="542271" cy="91440"/>
+          <a:off x="4242386" y="674335"/>
+          <a:ext cx="564116" cy="91440"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2686,13 +2701,13 @@
                 <a:pt x="0" y="45720"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="271135" y="45720"/>
+                <a:pt x="282058" y="45720"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="271135" y="77041"/>
+                <a:pt x="282058" y="78302"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="542271" y="77041"/>
+                <a:pt x="564116" y="78302"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -2746,8 +2761,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="4771227" y="678593"/>
-        <a:ext cx="27158" cy="27158"/>
+        <a:off x="4510317" y="705928"/>
+        <a:ext cx="28252" cy="28252"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{694BC8C3-6CEB-4210-BF0B-7306DFC930F3}">
@@ -2757,8 +2772,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2388399" y="692172"/>
-          <a:ext cx="542271" cy="1483179"/>
+          <a:off x="2031502" y="720055"/>
+          <a:ext cx="564116" cy="1542926"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2769,16 +2784,16 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="0" y="1483179"/>
+                <a:pt x="0" y="1542926"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="271135" y="1483179"/>
+                <a:pt x="282058" y="1542926"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="271135" y="0"/>
+                <a:pt x="282058" y="0"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="542271" y="0"/>
+                <a:pt x="564116" y="0"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -2832,8 +2847,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="2620055" y="1394281"/>
-        <a:ext cx="78960" cy="78960"/>
+        <a:off x="2272490" y="1450448"/>
+        <a:ext cx="82140" cy="82140"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{81D5B84E-6BE0-488C-832D-A8DA8D2C7D9C}">
@@ -2843,8 +2858,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm rot="16200000">
-          <a:off x="202606" y="1762034"/>
-          <a:ext cx="3544952" cy="826633"/>
+          <a:off x="-242341" y="1833015"/>
+          <a:ext cx="3687754" cy="859932"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2910,8 +2925,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="202606" y="1762034"/>
-        <a:ext cx="3544952" cy="826633"/>
+        <a:off x="-242341" y="1833015"/>
+        <a:ext cx="3687754" cy="859932"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{7976B0DA-7F78-450E-8AE3-662150B5EEAE}">
@@ -2921,8 +2936,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2930671" y="424706"/>
-          <a:ext cx="1582999" cy="534931"/>
+          <a:off x="2595618" y="441815"/>
+          <a:ext cx="1646767" cy="556479"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2988,8 +3003,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="2930671" y="424706"/>
-        <a:ext cx="1582999" cy="534931"/>
+        <a:off x="2595618" y="441815"/>
+        <a:ext cx="1646767" cy="556479"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{A21A6926-B908-4485-96D2-D69E2A0F3178}">
@@ -2999,8 +3014,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="5055942" y="479781"/>
-          <a:ext cx="2164341" cy="487424"/>
+          <a:off x="4806502" y="499108"/>
+          <a:ext cx="2251528" cy="507059"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3066,8 +3081,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="5055942" y="479781"/>
-        <a:ext cx="2164341" cy="487424"/>
+        <a:off x="4806502" y="499108"/>
+        <a:ext cx="2251528" cy="507059"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{807DB013-F690-4D56-A7B7-86955F551061}">
@@ -3077,8 +3092,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2930671" y="1166296"/>
-          <a:ext cx="1582999" cy="534931"/>
+          <a:off x="2595618" y="1213278"/>
+          <a:ext cx="1646767" cy="556479"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3144,8 +3159,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="2930671" y="1166296"/>
-        <a:ext cx="1582999" cy="534931"/>
+        <a:off x="2595618" y="1213278"/>
+        <a:ext cx="1646767" cy="556479"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{B2D62580-5B24-441B-90A9-7447F939058D}">
@@ -3155,8 +3170,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="5055942" y="1221370"/>
-          <a:ext cx="2164341" cy="487424"/>
+          <a:off x="4806502" y="1270571"/>
+          <a:ext cx="2251528" cy="507059"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3222,8 +3237,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="5055942" y="1221370"/>
-        <a:ext cx="2164341" cy="487424"/>
+        <a:off x="4806502" y="1270571"/>
+        <a:ext cx="2251528" cy="507059"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{7086A2D0-93F4-4D7D-90BB-E6B40AC5D9D0}">
@@ -3233,8 +3248,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2930671" y="1907885"/>
-          <a:ext cx="1582999" cy="534931"/>
+          <a:off x="2595618" y="1984741"/>
+          <a:ext cx="1646767" cy="556479"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3300,8 +3315,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="2930671" y="1907885"/>
-        <a:ext cx="1582999" cy="534931"/>
+        <a:off x="2595618" y="1984741"/>
+        <a:ext cx="1646767" cy="556479"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{C9821ED1-7E64-40C5-A2FB-435919AD4E5A}">
@@ -3311,8 +3326,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="5055942" y="1962960"/>
-          <a:ext cx="2164341" cy="487424"/>
+          <a:off x="4806502" y="2042034"/>
+          <a:ext cx="2251528" cy="507059"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3378,8 +3393,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="5055942" y="1962960"/>
-        <a:ext cx="2164341" cy="487424"/>
+        <a:off x="4806502" y="2042034"/>
+        <a:ext cx="2251528" cy="507059"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{833A11FC-3293-4373-B47B-79811B29138F}">
@@ -3389,8 +3404,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2930671" y="2649475"/>
-          <a:ext cx="1582999" cy="534931"/>
+          <a:off x="2595618" y="2756204"/>
+          <a:ext cx="1646767" cy="556479"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3456,8 +3471,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="2930671" y="2649475"/>
-        <a:ext cx="1582999" cy="534931"/>
+        <a:off x="2595618" y="2756204"/>
+        <a:ext cx="1646767" cy="556479"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{19597AE4-2372-4E4D-9E46-3BD6AAEACC16}">
@@ -3467,8 +3482,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="5055942" y="2673228"/>
-          <a:ext cx="2164341" cy="487424"/>
+          <a:off x="4806502" y="2780914"/>
+          <a:ext cx="2251528" cy="507059"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3534,8 +3549,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="5055942" y="2673228"/>
-        <a:ext cx="2164341" cy="487424"/>
+        <a:off x="4806502" y="2780914"/>
+        <a:ext cx="2251528" cy="507059"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{43DFBD47-131F-46CF-8189-37D4A2F57628}">
@@ -3545,8 +3560,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2930671" y="3391064"/>
-          <a:ext cx="1582999" cy="534931"/>
+          <a:off x="2595618" y="3527667"/>
+          <a:ext cx="1646767" cy="556479"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3612,8 +3627,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="2930671" y="3391064"/>
-        <a:ext cx="1582999" cy="534931"/>
+        <a:off x="2595618" y="3527667"/>
+        <a:ext cx="1646767" cy="556479"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{8D698A25-1CA2-47D5-B8DD-B0A9761A11BD}">
@@ -3623,8 +3638,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="5055942" y="3414818"/>
-          <a:ext cx="2164341" cy="487424"/>
+          <a:off x="4806502" y="3552377"/>
+          <a:ext cx="2251528" cy="507059"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3690,8 +3705,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="5055942" y="3414818"/>
-        <a:ext cx="2164341" cy="487424"/>
+        <a:off x="4806502" y="3552377"/>
+        <a:ext cx="2251528" cy="507059"/>
       </dsp:txXfrm>
     </dsp:sp>
   </dsp:spTree>
@@ -5121,8 +5136,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="8629650" y="3684270"/>
-          <a:ext cx="8951909" cy="4976470"/>
+          <a:off x="8077200" y="3733800"/>
+          <a:ext cx="8616629" cy="5182210"/>
           <a:chOff x="286808" y="1169878"/>
           <a:chExt cx="8616629" cy="5182210"/>
         </a:xfrm>
@@ -9697,19 +9712,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C2:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="5.26171875" customWidth="1"/>
-    <col min="4" max="4" width="91.83984375" customWidth="1"/>
-    <col min="5" max="5" width="11.41796875" customWidth="1"/>
-    <col min="8" max="8" width="84.578125" customWidth="1"/>
+    <col min="3" max="3" width="5.28515625" customWidth="1"/>
+    <col min="4" max="4" width="91.85546875" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" customWidth="1"/>
+    <col min="8" max="8" width="84.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C2" s="14" t="s">
         <v>0</v>
       </c>
@@ -9719,28 +9734,30 @@
       <c r="G2" s="14"/>
       <c r="H2" s="14"/>
     </row>
-    <row r="4" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
     </row>
-    <row r="5" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
     </row>
-    <row r="6" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
     </row>
-    <row r="7" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
     </row>
-    <row r="9" spans="3:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
-    <row r="10" spans="3:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="9" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F9" s="17"/>
+    </row>
+    <row r="10" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C10" s="1" t="s">
         <v>1</v>
       </c>
@@ -9760,166 +9777,184 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="3:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="11" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C11" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E11" s="3"/>
       <c r="F11" s="3" t="s">
         <v>12</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>31</v>
+        <v>58</v>
       </c>
     </row>
-    <row r="12" spans="3:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="12" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H12" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>35</v>
+    </row>
+    <row r="13" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C13" s="3" t="s">
+        <v>34</v>
       </c>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="3:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="C13" s="3" t="s">
+      <c r="D13" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>32</v>
+      <c r="E13" s="3" t="s">
+        <v>44</v>
       </c>
-      <c r="E13" s="3"/>
       <c r="F13" s="3" t="s">
         <v>12</v>
       </c>
       <c r="G13" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C14" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F14" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H13" s="3" t="s">
+      <c r="G14" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C15" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H15" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="3:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="C14" s="3" t="s">
-        <v>47</v>
+    <row r="16" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C16" s="3" t="s">
+        <v>37</v>
       </c>
-      <c r="D14" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="3:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="C15" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="3:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="C16" s="3" t="s">
+      <c r="D16" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>34</v>
+      <c r="E16" s="3" t="s">
+        <v>44</v>
       </c>
-      <c r="E16" s="3"/>
       <c r="F16" s="3" t="s">
         <v>12</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
     </row>
-    <row r="17" spans="3:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="17" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C17" s="3" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
-      <c r="E17" s="3"/>
+      <c r="E17" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="F17" s="3" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
     </row>
-    <row r="18" spans="3:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="18" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C18" s="3" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
-      <c r="E18" s="3"/>
+      <c r="E18" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="F18" s="3" t="s">
         <v>12</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
     </row>
-    <row r="19" spans="3:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="19" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C19" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D19" s="3" t="s">
-        <v>55</v>
+      <c r="E19" s="3" t="s">
+        <v>42</v>
       </c>
-      <c r="E19" s="3"/>
       <c r="F19" s="3" t="s">
         <v>12</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -9938,19 +9973,19 @@
       <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="8.68359375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.15625" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="15"/>
       <c r="C1" s="15"/>
       <c r="D1" s="15"/>
     </row>
-    <row r="2" spans="2:16" ht="26.1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="2" spans="2:16" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="4" t="s">
         <v>21</v>
       </c>
@@ -9961,7 +9996,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="2:16" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="3" spans="2:16" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="s">
         <v>9</v>
       </c>
@@ -9972,7 +10007,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="2:16" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="4" spans="2:16" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="10" t="s">
         <v>12</v>
       </c>
@@ -9983,7 +10018,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="2:16" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="5" spans="2:16" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="13" t="s">
         <v>15</v>
       </c>
@@ -9994,7 +10029,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="2:16" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="6" spans="2:16" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="7" t="s">
         <v>18</v>
       </c>
@@ -10005,7 +10040,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="J9" s="16" t="s">
         <v>22</v>
       </c>

</xml_diff>